<commit_message>
Fixed Override Currency List in template
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/NavQuarterlyUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/NavQuarterlyUploadTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvanumamalai\Documents\SQL Server Management Studio\AC-379\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvanumamalai\source\repos\Ark-WebUI New\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4375418C-0B88-499E-A788-C422CA8E2575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5HNAWO4E28XRrPb67oYf4tgxOTknr9pLTvHtDovVwkitrb7meLqE9Pw5nlX7A+/GVL/VCxuQ39YmKO6eX1bxRg==" workbookSaltValue="aLdH3xi2FjF7n7oZ2SLcYQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954A5F5C-B017-4A80-936C-F82E0C979A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Yx1q4o1BkIXou/AoFH/a5UACtGmtogtTTximr2qFBt9/BKorPruoCb8vfva+a9KJLpdb76+lTzwnYBFl5ZueSA==" workbookSaltValue="dbdhjBguXaNRzIzChjubuQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{C4DEDF0A-76DA-43B5-A336-FA0AFA6A6B16}"/>
   </bookViews>
@@ -745,7 +745,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,7 +846,7 @@
       <c r="R2" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4FWK+4NLDQqths1/ACxByeQHivr9OmvqB/l3CEQxCvdktrlS63MzFNVfyP9PxmF8oWVoFlV7YFI7qc9JwgDSbw==" saltValue="bZ8AgdA15tM2GceFYTWSJw==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="rFyyJ2sYEK+MX2ihwFIONx9UZNa5ry7qxgj+N2IAIVAPpdKBLF23P1G1fS5pjRIeWB+V8Dwov4NLb8lIVnBNWA==" saltValue="6ULMooptVzj7RCwQTOp9Lg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <dataValidations count="6">
     <dataValidation type="date" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{D08F1287-6FDD-4FAF-A6E4-DE6D102FCAB3}">
       <formula1>40909</formula1>
@@ -887,7 +887,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E3054ACC-70E9-409A-8F2C-027545954C36}">
           <x14:formula1>
-            <xm:f>Sheet2!$C$1:$C$5</xm:f>
+            <xm:f>Sheet2!$D$1:$D$7</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
@@ -902,7 +902,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
@@ -1265,6 +1265,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="e71fa759-47f8-4a70-96bd-5964b1ae8857">
+      <UserInfo>
+        <DisplayName>Jean Wai</DisplayName>
+        <AccountId>29</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Shubh Gosalia</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010017EB258DADFA3746A36EC080AC089D83" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7ebb95de695edb82866e27aa90a207c8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5e1f9c12-bc96-4798-a342-bb349a93830a" xmlns:ns3="e71fa759-47f8-4a70-96bd-5964b1ae8857" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3e86bd6f45c4d31b841dbab4160863d0" ns2:_="" ns3:_="">
     <xsd:import namespace="5e1f9c12-bc96-4798-a342-bb349a93830a"/>
@@ -1435,35 +1463,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C53ECC68-04E7-452A-99A3-10030F701C32}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e71fa759-47f8-4a70-96bd-5964b1ae8857"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="e71fa759-47f8-4a70-96bd-5964b1ae8857">
-      <UserInfo>
-        <DisplayName>Jean Wai</DisplayName>
-        <AccountId>29</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Shubh Gosalia</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D307A0-5037-428A-99CA-08384DEEE293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F57BD9C-43FE-499F-B6CD-EF500BF99DC9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1480,22 +1498,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D307A0-5037-428A-99CA-08384DEEE293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C53ECC68-04E7-452A-99A3-10030F701C32}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e71fa759-47f8-4a70-96bd-5964b1ae8857"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed validation for bulk upload templates
</commit_message>
<xml_diff>
--- a/ArkWebApp/src/assets/files/templates/NavQuarterlyUploadTemplate.xlsx
+++ b/ArkWebApp/src/assets/files/templates/NavQuarterlyUploadTemplate.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvanumamalai\source\repos\Ark-WebUI New\Ark-WebUI\ArkWebApp\src\assets\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954A5F5C-B017-4A80-936C-F82E0C979A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Yx1q4o1BkIXou/AoFH/a5UACtGmtogtTTximr2qFBt9/BKorPruoCb8vfva+a9KJLpdb76+lTzwnYBFl5ZueSA==" workbookSaltValue="dbdhjBguXaNRzIzChjubuQ==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D734428F-0485-4149-B864-AB8DDBC4882D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ubWoHni5nAVAeY6zs2mwarbOdkh4+p9/55Y2B51ZxM/HThZ1DdHaPxV0kwwzUVr2LOntG4Uyvq9WGwsgOvSlbQ==" workbookSaltValue="YWounfiIVYWMwsj72rAwOQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{C4DEDF0A-76DA-43B5-A336-FA0AFA6A6B16}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C4DEDF0A-76DA-43B5-A336-FA0AFA6A6B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
@@ -409,19 +409,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -742,10 +729,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E9AB30-9C00-4DA9-B8B8-8591DD4EBC6B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,45 +813,26 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rFyyJ2sYEK+MX2ihwFIONx9UZNa5ry7qxgj+N2IAIVAPpdKBLF23P1G1fS5pjRIeWB+V8Dwov4NLb8lIVnBNWA==" saltValue="6ULMooptVzj7RCwQTOp9Lg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="3FhMqWCh01Ejvi4WHO/NKXs+0oqw22pi3QELNBIaxEGpCKMbbXepocAP949sVHFtP26A30WUbp6LDHtTYNgE9Q==" saltValue="Zlc8S1uoG4PgCBKbxXakuw==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <dataValidations count="6">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H2:I1048576 E2:F1048576" xr:uid="{BF3B5D86-28C3-4CAD-8483-DF2A4EA30B61}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:M1048576 P2:P1048576" xr:uid="{E1AA2747-7A12-47ED-B962-D6D2B0DAED02}">
+      <formula1>0</formula1>
+    </dataValidation>
     <dataValidation type="date" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{D08F1287-6FDD-4FAF-A6E4-DE6D102FCAB3}">
       <formula1>40909</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576 Q2:Q1048576 R2:R1048576 N2:N1048576" xr:uid="{036B4034-F449-4ED6-8518-CAFB951D49DA}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:R1048576 N2:O1048576" xr:uid="{036B4034-F449-4ED6-8518-CAFB951D49DA}">
       <formula1>-99999999999</formula1>
       <formula2>99999999999</formula2>
     </dataValidation>
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{6A740DF4-617F-45B1-AB9D-D59292EBC1EC}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" sqref="H2:I1048576 E2:F1048576" xr:uid="{BF3B5D86-28C3-4CAD-8483-DF2A4EA30B61}">
-      <formula1>0</formula1>
-    </dataValidation>
     <dataValidation type="decimal" errorStyle="information" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{B5386FCD-9C79-4616-9156-3C064D160E5B}">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576 K2:K1048576 L2:L1048576 P2:P1048576" xr:uid="{E1AA2747-7A12-47ED-B962-D6D2B0DAED02}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -1225,37 +1193,37 @@
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="8" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="8" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1265,34 +1233,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="e71fa759-47f8-4a70-96bd-5964b1ae8857">
-      <UserInfo>
-        <DisplayName>Jean Wai</DisplayName>
-        <AccountId>29</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Shubh Gosalia</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010017EB258DADFA3746A36EC080AC089D83" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7ebb95de695edb82866e27aa90a207c8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5e1f9c12-bc96-4798-a342-bb349a93830a" xmlns:ns3="e71fa759-47f8-4a70-96bd-5964b1ae8857" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3e86bd6f45c4d31b841dbab4160863d0" ns2:_="" ns3:_="">
     <xsd:import namespace="5e1f9c12-bc96-4798-a342-bb349a93830a"/>
@@ -1463,25 +1403,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C53ECC68-04E7-452A-99A3-10030F701C32}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e71fa759-47f8-4a70-96bd-5964b1ae8857"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D307A0-5037-428A-99CA-08384DEEE293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="e71fa759-47f8-4a70-96bd-5964b1ae8857">
+      <UserInfo>
+        <DisplayName>Jean Wai</DisplayName>
+        <AccountId>29</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Shubh Gosalia</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F57BD9C-43FE-499F-B6CD-EF500BF99DC9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1498,4 +1448,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D307A0-5037-428A-99CA-08384DEEE293}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C53ECC68-04E7-452A-99A3-10030F701C32}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e71fa759-47f8-4a70-96bd-5964b1ae8857"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>